<commit_message>
Added more struggle data and repaired falling data
</commit_message>
<xml_diff>
--- a/spliced/falling/2023-03-21_15-34-18/accelerometer_selected.xlsx
+++ b/spliced/falling/2023-03-21_15-34-18/accelerometer_selected.xlsx
@@ -452,222 +452,222 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.3787193298339841</v>
+        <v>0.1436797380447386</v>
       </c>
       <c r="B2" t="n">
-        <v>0.750096321105957</v>
+        <v>0.7403357923030853</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.375997304916381</v>
+        <v>-1.325827866792679</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1436797380447386</v>
+        <v>-1.716686248779299</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7403357923030853</v>
+        <v>1.053612291812897</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.325827866792679</v>
+        <v>0.4070562124252333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1.716686248779299</v>
+        <v>-3.969705402851109</v>
       </c>
       <c r="B4" t="n">
-        <v>1.053612291812897</v>
+        <v>0.09983259439468162</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4070562124252333</v>
+        <v>0.9274015724658967</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-3.969705402851109</v>
+        <v>-5.239097833633425</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09983259439468162</v>
+        <v>-0.5959589481353762</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9274015724658967</v>
+        <v>-0.1143757104873694</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-5.239097833633425</v>
+        <v>2.036354780197156</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.5959589481353762</v>
+        <v>-0.2977316975593562</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.1143757104873694</v>
+        <v>-1.156379550695419</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.036354780197156</v>
+        <v>5.741946458816498</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.2977316975593562</v>
+        <v>-4.677600264549274</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.156379550695419</v>
+        <v>-8.871290028095274</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5.741946458816498</v>
+        <v>-18.10554087162019</v>
       </c>
       <c r="B8" t="n">
-        <v>-4.677600264549274</v>
+        <v>-17.49406802654266</v>
       </c>
       <c r="C8" t="n">
-        <v>-8.871290028095274</v>
+        <v>-29.53683829307556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-18.10554087162019</v>
+        <v>1.688319206237781</v>
       </c>
       <c r="B9" t="n">
-        <v>-17.49406802654266</v>
+        <v>-2.673514366149895</v>
       </c>
       <c r="C9" t="n">
-        <v>-29.53683829307556</v>
+        <v>-12.34325218200682</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.688319206237781</v>
+        <v>-3.507262408733383</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.673514366149895</v>
+        <v>0.2684899270534595</v>
       </c>
       <c r="C10" t="n">
-        <v>-12.34325218200682</v>
+        <v>-2.699394106864903</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-3.507262408733383</v>
+        <v>-0.7152169942855791</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2684899270534595</v>
+        <v>0.4368197321891781</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.699394106864903</v>
+        <v>0.5279676914215112</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.7152169942855791</v>
+        <v>0.77803122997284</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4368197321891781</v>
+        <v>0.2878375947475432</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5279676914215112</v>
+        <v>-0.8067402243614243</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.77803122997284</v>
+        <v>-0.02435183525085627</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2878375947475432</v>
+        <v>-0.3931519985198989</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.8067402243614243</v>
+        <v>-2.55875074863434</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-0.02435183525085627</v>
+        <v>-0.2728092074394176</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.3931519985198989</v>
+        <v>-0.8767854124307625</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.55875074863434</v>
+        <v>-2.626779749989506</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.2728092074394176</v>
+        <v>1.066039085388185</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.8767854124307625</v>
+        <v>-0.5432969331741325</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.626779749989506</v>
+        <v>-1.81298840045929</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.066039085388185</v>
+        <v>1.15899240970611</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.5432969331741325</v>
+        <v>-0.2723855525255186</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.81298840045929</v>
+        <v>-1.873978555202483</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.15899240970611</v>
+        <v>-0.3004360198974618</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2723855525255186</v>
+        <v>0.163273096084592</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.873978555202483</v>
+        <v>-1.427715420722963</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-0.3004360198974618</v>
+        <v>-0.5053797960281373</v>
       </c>
       <c r="B18" t="n">
-        <v>0.163273096084592</v>
+        <v>-0.4524855315685276</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.427715420722963</v>
+        <v>-1.996987149119378</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.5053797960281373</v>
+        <v>0.1984210014343271</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.4524855315685276</v>
+        <v>-0.3136261999607083</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.996987149119378</v>
+        <v>-1.604727536439895</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1984210014343271</v>
+        <v>0.1348390579223627</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.3136261999607083</v>
+        <v>-0.3085210472345353</v>
       </c>
       <c r="C20" t="n">
-        <v>-1.604727536439895</v>
+        <v>-1.704802349209786</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1348390579223627</v>
+        <v>-0.11956262588501</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3085210472345353</v>
+        <v>-0.3192775845527647</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.704802349209786</v>
+        <v>-1.924065947532654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>